<commit_message>
Cleaned up mounted pipeline so to remove seperate Trim folder
</commit_message>
<xml_diff>
--- a/Person_B_and_trucks/on_trucks/Processed_Standalone/10_245-70R19.xlsx
+++ b/Person_B_and_trucks/on_trucks/Processed_Standalone/10_245-70R19.xlsx
@@ -1043,100 +1043,100 @@
         <v>0</v>
       </c>
       <c r="AR2">
-        <v>0.1883562720413256</v>
+        <v>0.1582799338574765</v>
       </c>
       <c r="AS2">
-        <v>0.02510516389178956</v>
+        <v>0.02976356826885447</v>
       </c>
       <c r="AT2">
-        <v>0.2806140951908258</v>
+        <v>0.2309081705824061</v>
       </c>
       <c r="AU2">
-        <v>0</v>
+        <v>0.007435948128591326</v>
       </c>
       <c r="AV2">
-        <v>0</v>
+        <v>0.009759633217620085</v>
       </c>
       <c r="AW2">
-        <v>0.01799627644658349</v>
+        <v>0.02416723028259336</v>
       </c>
       <c r="AX2">
-        <v>0.09188788860966107</v>
+        <v>0.08233701271362144</v>
       </c>
       <c r="AY2">
-        <v>0</v>
+        <v>0.005042146156178672</v>
       </c>
       <c r="AZ2">
-        <v>0.01772962084126473</v>
+        <v>0.02395731067072763</v>
       </c>
       <c r="BA2">
-        <v>0.08651575188835429</v>
+        <v>0.07810789908190803</v>
       </c>
       <c r="BB2">
-        <v>0.007515628400145689</v>
+        <v>0.01591653715585574</v>
       </c>
       <c r="BC2">
-        <v>0</v>
+        <v>0.001200630701436203</v>
       </c>
       <c r="BD2">
-        <v>0</v>
+        <v>0.001510895475352135</v>
       </c>
       <c r="BE2">
-        <v>0.0679215628021367</v>
+        <v>0.06346997331518424</v>
       </c>
       <c r="BF2">
-        <v>0.009354707817189264</v>
+        <v>0.01736431785018822</v>
       </c>
       <c r="BG2">
-        <v>0.009409078027060314</v>
+        <v>0.01740711977568889</v>
       </c>
       <c r="BH2">
-        <v>0.06249699576466432</v>
+        <v>0.05919958490281763</v>
       </c>
       <c r="BI2">
-        <v>0</v>
+        <v>0.001692714321858239</v>
       </c>
       <c r="BJ2">
-        <v>0.0009130098233818617</v>
+        <v>0.01071874981785892</v>
       </c>
       <c r="BK2">
-        <v>0.08538596395270243</v>
+        <v>0.07721849477083376</v>
       </c>
       <c r="BL2">
-        <v>0.01451133998321967</v>
+        <v>0.02142377957248523</v>
       </c>
       <c r="BM2">
-        <v>0.02045269134469629</v>
+        <v>0.02610099672780508</v>
       </c>
       <c r="BN2">
-        <v>0</v>
+        <v>9.364172999275077E-06</v>
       </c>
       <c r="BO2">
-        <v>0</v>
+        <v>0.0002255233741107637</v>
       </c>
       <c r="BP2">
-        <v>0</v>
+        <v>0.00642212007671395</v>
       </c>
       <c r="BQ2">
-        <v>0</v>
+        <v>0.001176847128283185</v>
       </c>
       <c r="BR2">
-        <v>0</v>
+        <v>0.001009274229347933</v>
       </c>
       <c r="BS2">
-        <v>0</v>
+        <v>0.001135935292444357</v>
       </c>
       <c r="BT2">
-        <v>0</v>
+        <v>0.0003288726482394361</v>
       </c>
       <c r="BU2">
-        <v>0</v>
+        <v>0.001218978784841863</v>
       </c>
       <c r="BV2">
-        <v>0</v>
+        <v>0.004599917402339626</v>
       </c>
       <c r="BW2">
-        <v>0.0138339531749992</v>
+        <v>0.02089051954333781</v>
       </c>
     </row>
     <row r="3" spans="1:75">
@@ -1270,100 +1270,100 @@
         <v>0</v>
       </c>
       <c r="AR3">
-        <v>0.2810718858277978</v>
+        <v>0.2359324336513552</v>
       </c>
       <c r="AS3">
-        <v>0.09570109906500639</v>
+        <v>0.08692687637963657</v>
       </c>
       <c r="AT3">
-        <v>0.3081852082731207</v>
+        <v>0.2577267831872556</v>
       </c>
       <c r="AU3">
-        <v>0</v>
+        <v>0.006894872849615351</v>
       </c>
       <c r="AV3">
-        <v>0</v>
+        <v>0.001430526072309883</v>
       </c>
       <c r="AW3">
-        <v>0.0043345091647187</v>
+        <v>0.01348418413099125</v>
       </c>
       <c r="AX3">
-        <v>0.1147149655833565</v>
+        <v>0.102210685797149</v>
       </c>
       <c r="AY3">
-        <v>0.00793617876372193</v>
+        <v>0.01637929395428196</v>
       </c>
       <c r="AZ3">
-        <v>0.02655650898660795</v>
+        <v>0.03134676930407895</v>
       </c>
       <c r="BA3">
-        <v>0.01184477026260017</v>
+        <v>0.01952111508267325</v>
       </c>
       <c r="BB3">
-        <v>0</v>
+        <v>0.000781438912351826</v>
       </c>
       <c r="BC3">
-        <v>0</v>
+        <v>0.001237464920465276</v>
       </c>
       <c r="BD3">
-        <v>0.002125668525927968</v>
+        <v>0.01170866417957302</v>
       </c>
       <c r="BE3">
-        <v>0.007929201533682935</v>
+        <v>0.01637368548668936</v>
       </c>
       <c r="BF3">
-        <v>0.02547915724157416</v>
+        <v>0.03048076770830517</v>
       </c>
       <c r="BG3">
-        <v>0</v>
+        <v>0.001086670994902704</v>
       </c>
       <c r="BH3">
-        <v>0.01472853565955751</v>
+        <v>0.02183915600766747</v>
       </c>
       <c r="BI3">
-        <v>0</v>
+        <v>0.003011790692456108</v>
       </c>
       <c r="BJ3">
-        <v>0</v>
+        <v>0.0002575385460480553</v>
       </c>
       <c r="BK3">
-        <v>0.06350268928220477</v>
+        <v>0.06104500968027951</v>
       </c>
       <c r="BL3">
-        <v>0</v>
+        <v>0.006996789545668194</v>
       </c>
       <c r="BM3">
-        <v>0.005367150936926981</v>
+        <v>0.01431424676069163</v>
       </c>
       <c r="BN3">
-        <v>0</v>
+        <v>2.502827914025464E-06</v>
       </c>
       <c r="BO3">
-        <v>0</v>
+        <v>2.423670285203422E-05</v>
       </c>
       <c r="BP3">
-        <v>0</v>
+        <v>0.002726218598186293</v>
       </c>
       <c r="BQ3">
-        <v>0</v>
+        <v>0.002417979340146228</v>
       </c>
       <c r="BR3">
-        <v>0</v>
+        <v>0.0001649385421000762</v>
       </c>
       <c r="BS3">
-        <v>0</v>
+        <v>0.0005709664378209294</v>
       </c>
       <c r="BT3">
-        <v>0</v>
+        <v>0.002363171179722317</v>
       </c>
       <c r="BU3">
-        <v>0</v>
+        <v>0.006208516362079939</v>
       </c>
       <c r="BV3">
-        <v>0.008915787724415331</v>
+        <v>0.01716672751728061</v>
       </c>
       <c r="BW3">
-        <v>0.02160668316878013</v>
+        <v>0.02736797864745204</v>
       </c>
     </row>
     <row r="4" spans="1:75">
@@ -1497,100 +1497,100 @@
         <v>0</v>
       </c>
       <c r="AR4">
-        <v>0.2847639121176406</v>
+        <v>0.2412224171542024</v>
       </c>
       <c r="AS4">
-        <v>0.1407597575663971</v>
+        <v>0.1242940168945855</v>
       </c>
       <c r="AT4">
-        <v>0.2709178435558056</v>
+        <v>0.2299796953600599</v>
       </c>
       <c r="AU4">
-        <v>0</v>
+        <v>0.001079146618584842</v>
       </c>
       <c r="AV4">
-        <v>0</v>
+        <v>0.00202767267402883</v>
       </c>
       <c r="AW4">
-        <v>0</v>
+        <v>0.001382593649543406</v>
       </c>
       <c r="AX4">
-        <v>0.1238003093150366</v>
+        <v>0.1105232950741142</v>
       </c>
       <c r="AY4">
-        <v>0.01895901933885585</v>
+        <v>0.02539433225862033</v>
       </c>
       <c r="AZ4">
-        <v>0.03177633361973534</v>
+        <v>0.03580172681718962</v>
       </c>
       <c r="BA4">
-        <v>0.004106824489686503</v>
+        <v>0.01333465669252745</v>
       </c>
       <c r="BB4">
-        <v>0</v>
+        <v>4.113125218718544E-05</v>
       </c>
       <c r="BC4">
-        <v>0</v>
+        <v>0.0006660989829517935</v>
       </c>
       <c r="BD4">
-        <v>0.003039826768261577</v>
+        <v>0.01246827657290057</v>
       </c>
       <c r="BE4">
-        <v>0</v>
+        <v>0.005643537232047784</v>
       </c>
       <c r="BF4">
-        <v>0.01598442663664308</v>
+        <v>0.02297902440047168</v>
       </c>
       <c r="BG4">
-        <v>0</v>
+        <v>0.005064990458729038</v>
       </c>
       <c r="BH4">
-        <v>0.004849594737302712</v>
+        <v>0.01393777079770625</v>
       </c>
       <c r="BI4">
-        <v>0</v>
+        <v>0.001519505444166734</v>
       </c>
       <c r="BJ4">
-        <v>0</v>
+        <v>0.004490230564271972</v>
       </c>
       <c r="BK4">
-        <v>0.06836687521874248</v>
+        <v>0.06551249111519039</v>
       </c>
       <c r="BL4">
-        <v>0</v>
+        <v>0.006808395252841702</v>
       </c>
       <c r="BM4">
-        <v>0</v>
+        <v>0.007899619783207261</v>
       </c>
       <c r="BN4">
-        <v>0</v>
+        <v>0.0008634232988327312</v>
       </c>
       <c r="BO4">
-        <v>0</v>
+        <v>0.001804315183125061</v>
       </c>
       <c r="BP4">
-        <v>0</v>
+        <v>0.0004398175871438931</v>
       </c>
       <c r="BQ4">
-        <v>0</v>
+        <v>0.002157522184236378</v>
       </c>
       <c r="BR4">
-        <v>0</v>
+        <v>0.001116734703165016</v>
       </c>
       <c r="BS4">
-        <v>0</v>
+        <v>0.00131318468325835</v>
       </c>
       <c r="BT4">
-        <v>0</v>
+        <v>0.003702727324166083</v>
       </c>
       <c r="BU4">
-        <v>0.000849403767639064</v>
+        <v>0.01068969832178824</v>
       </c>
       <c r="BV4">
-        <v>0.01497005020782152</v>
+        <v>0.02215537168397342</v>
       </c>
       <c r="BW4">
-        <v>0.01685582266043188</v>
+        <v>0.02368657998018211</v>
       </c>
     </row>
     <row r="5" spans="1:75">
@@ -1724,100 +1724,100 @@
         <v>0</v>
       </c>
       <c r="AR5">
-        <v>0.2016516135182773</v>
+        <v>0.1696070221949173</v>
       </c>
       <c r="AS5">
-        <v>0.04034648798539808</v>
+        <v>0.04193419924105256</v>
       </c>
       <c r="AT5">
-        <v>0.3233782875579669</v>
+        <v>0.2659535459156672</v>
       </c>
       <c r="AU5">
-        <v>0.007408307741336323</v>
+        <v>0.01586366713099011</v>
       </c>
       <c r="AV5">
-        <v>0</v>
+        <v>0.003169019478353818</v>
       </c>
       <c r="AW5">
-        <v>0.03172615759207197</v>
+        <v>0.03511121756285034</v>
       </c>
       <c r="AX5">
-        <v>0.1075433285689083</v>
+        <v>0.09512042195118491</v>
       </c>
       <c r="AY5">
-        <v>0.01045456113914201</v>
+        <v>0.01827477322229271</v>
       </c>
       <c r="AZ5">
-        <v>0.03323315708005286</v>
+        <v>0.03630400593944369</v>
       </c>
       <c r="BA5">
-        <v>0.02547289721365328</v>
+        <v>0.03016176910272976</v>
       </c>
       <c r="BB5">
-        <v>0</v>
+        <v>0.001573306140093603</v>
       </c>
       <c r="BC5">
-        <v>0</v>
+        <v>0.001788213036622541</v>
       </c>
       <c r="BD5">
-        <v>0</v>
+        <v>0.003890138463041729</v>
       </c>
       <c r="BE5">
-        <v>0.02467773573741563</v>
+        <v>0.02953239970085833</v>
       </c>
       <c r="BF5">
-        <v>0.01150139106056939</v>
+        <v>0.01910333791160237</v>
       </c>
       <c r="BG5">
-        <v>0</v>
+        <v>0.004439076341898951</v>
       </c>
       <c r="BH5">
-        <v>0.03517353274975801</v>
+        <v>0.03783981106977575</v>
       </c>
       <c r="BI5">
-        <v>0</v>
+        <v>0.000309854482794494</v>
       </c>
       <c r="BJ5">
-        <v>0</v>
+        <v>0.001083251065675064</v>
       </c>
       <c r="BK5">
-        <v>0.09222974245457435</v>
+        <v>0.08299973600084541</v>
       </c>
       <c r="BL5">
-        <v>0.01130436783930669</v>
+        <v>0.01894739425660086</v>
       </c>
       <c r="BM5">
-        <v>0.02186882985574325</v>
+        <v>0.02730915389797324</v>
       </c>
       <c r="BN5">
-        <v>0</v>
+        <v>0.0001126782219415111</v>
       </c>
       <c r="BO5">
-        <v>0</v>
+        <v>0.0007971241205287643</v>
       </c>
       <c r="BP5">
-        <v>0</v>
+        <v>0.006791007693432307</v>
       </c>
       <c r="BQ5">
-        <v>0</v>
+        <v>0.00525613301017086</v>
       </c>
       <c r="BR5">
-        <v>0</v>
+        <v>0.0001682312527507867</v>
       </c>
       <c r="BS5">
-        <v>0</v>
+        <v>0.0004296298331455021</v>
       </c>
       <c r="BT5">
-        <v>0</v>
+        <v>0.003281377798315111</v>
       </c>
       <c r="BU5">
-        <v>0</v>
+        <v>0.005412099170134015</v>
       </c>
       <c r="BV5">
-        <v>0.003305170023756752</v>
+        <v>0.01261603830554971</v>
       </c>
       <c r="BW5">
-        <v>0.01872443188206918</v>
+        <v>0.02482036648676633</v>
       </c>
     </row>
     <row r="6" spans="1:75">
@@ -1948,100 +1948,100 @@
         <v>0</v>
       </c>
       <c r="AQ6">
-        <v>0.005630125271338065</v>
+        <v>0.01453263636904105</v>
       </c>
       <c r="AR6">
-        <v>0.2212141198256587</v>
+        <v>0.1880925142059736</v>
       </c>
       <c r="AS6">
-        <v>0.2265284776502698</v>
+        <v>0.1923709361580673</v>
       </c>
       <c r="AT6">
-        <v>0.1807452827802943</v>
+        <v>0.1555123292608135</v>
       </c>
       <c r="AU6">
-        <v>0</v>
+        <v>0.001244872732292092</v>
       </c>
       <c r="AV6">
-        <v>0</v>
+        <v>0.002681351633310149</v>
       </c>
       <c r="AW6">
-        <v>0.005106432762393669</v>
+        <v>0.01411102803923712</v>
       </c>
       <c r="AX6">
-        <v>0.1973088537913883</v>
+        <v>0.1688471381234652</v>
       </c>
       <c r="AY6">
-        <v>0.01555486107933129</v>
+        <v>0.0225227282956711</v>
       </c>
       <c r="AZ6">
-        <v>0.003096913791262934</v>
+        <v>0.01249322766467096</v>
       </c>
       <c r="BA6">
-        <v>0</v>
+        <v>0.008536265613997495</v>
       </c>
       <c r="BB6">
-        <v>0</v>
+        <v>0.0002406732964225959</v>
       </c>
       <c r="BC6">
-        <v>0</v>
+        <v>0.003080565638346547</v>
       </c>
       <c r="BD6">
-        <v>0.009917407698003351</v>
+        <v>0.01798419229629224</v>
       </c>
       <c r="BE6">
-        <v>0</v>
+        <v>0.0001179116541926458</v>
       </c>
       <c r="BF6">
-        <v>0</v>
+        <v>0.008898425159575995</v>
       </c>
       <c r="BG6">
-        <v>0.01354812936084224</v>
+        <v>0.02090717185034</v>
       </c>
       <c r="BH6">
-        <v>0</v>
+        <v>0.005407179719341838</v>
       </c>
       <c r="BI6">
-        <v>0</v>
+        <v>0.00171898118371056</v>
       </c>
       <c r="BJ6">
-        <v>0.01871049013293005</v>
+        <v>0.02506322576707905</v>
       </c>
       <c r="BK6">
-        <v>0.0824615938098706</v>
+        <v>0.07638722961538641</v>
       </c>
       <c r="BL6">
-        <v>0</v>
+        <v>2.113758153013928E-06</v>
       </c>
       <c r="BM6">
-        <v>0</v>
+        <v>0.006020800331356083</v>
       </c>
       <c r="BN6">
-        <v>0</v>
+        <v>0.001199061936805612</v>
       </c>
       <c r="BO6">
-        <v>0</v>
+        <v>0.0001740231645584444</v>
       </c>
       <c r="BP6">
-        <v>0</v>
+        <v>0.002126642536586437</v>
       </c>
       <c r="BQ6">
-        <v>0</v>
+        <v>0.003547765944820098</v>
       </c>
       <c r="BR6">
-        <v>0</v>
+        <v>0.00156803990294849</v>
       </c>
       <c r="BS6">
-        <v>0</v>
+        <v>2.853432736955325E-05</v>
       </c>
       <c r="BT6">
-        <v>0</v>
+        <v>0.008338315971382425</v>
       </c>
       <c r="BU6">
-        <v>0.002053884637459715</v>
+        <v>0.01165351777392194</v>
       </c>
       <c r="BV6">
-        <v>0.01812342740895694</v>
+        <v>0.02459060007487017</v>
       </c>
       <c r="BW6">
         <v>0</v>
@@ -2058,22 +2058,22 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.002056664043484111</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0.129334167665091</v>
+        <v>0.1405024519496363</v>
       </c>
       <c r="F7">
-        <v>0.02072565488618068</v>
+        <v>0.01281764374176696</v>
       </c>
       <c r="G7">
-        <v>0.2755030635257049</v>
+        <v>0.3123448513747267</v>
       </c>
       <c r="H7">
-        <v>0.06612825498102003</v>
+        <v>0.06619488035902286</v>
       </c>
       <c r="I7">
-        <v>0.02041544467279583</v>
+        <v>0.0124529473603627</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -2085,25 +2085,25 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>0.2405682824292601</v>
+        <v>0.2712740300371416</v>
       </c>
       <c r="N7">
-        <v>0.04740479292504285</v>
+        <v>0.04418277835674781</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7">
-        <v>0.05875091417251681</v>
+        <v>0.057521763288215</v>
       </c>
       <c r="Q7">
-        <v>0.009822985698967083</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <v>0.01983851680862085</v>
+        <v>0.0117746863124749</v>
       </c>
       <c r="S7">
-        <v>0.01339703983617692</v>
+        <v>0.004201810754587505</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -2115,13 +2115,13 @@
         <v>0</v>
       </c>
       <c r="W7">
-        <v>0.02581443201604547</v>
+        <v>0.01880022756705204</v>
       </c>
       <c r="X7">
-        <v>0.02574345689215807</v>
+        <v>0.01871678617881078</v>
       </c>
       <c r="Y7">
-        <v>0.01037491380084151</v>
+        <v>0.0006488702591465145</v>
       </c>
       <c r="Z7">
         <v>0</v>
@@ -2151,7 +2151,7 @@
         <v>0</v>
       </c>
       <c r="AI7">
-        <v>0.03412141564609376</v>
+        <v>0.02856627246030824</v>
       </c>
       <c r="AJ7">
         <v>0</v>
@@ -2288,46 +2288,46 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0.1714552967088327</v>
+        <v>0.1564184647388446</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.0006257720422178086</v>
       </c>
       <c r="G8">
-        <v>0.1268710911921427</v>
+        <v>0.1175769189423239</v>
       </c>
       <c r="H8">
-        <v>0.1378342289241996</v>
+        <v>0.1271279519002589</v>
       </c>
       <c r="I8">
-        <v>0.06823849261464773</v>
+        <v>0.06649648055783257</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>0.000632564968630007</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>0.002658185090607857</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>0.0009411345246219961</v>
       </c>
       <c r="M8">
-        <v>0.153850546015204</v>
+        <v>0.1410812904552987</v>
       </c>
       <c r="N8">
-        <v>0.03204187273025869</v>
+        <v>0.03496215909521413</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8">
-        <v>0.08062121855260755</v>
+        <v>0.07728425194528016</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
       <c r="R8">
-        <v>0.06660888750725841</v>
+        <v>0.06507677641204014</v>
       </c>
       <c r="S8">
         <v>0</v>
@@ -2336,22 +2336,22 @@
         <v>0</v>
       </c>
       <c r="U8">
-        <v>0.008471117633059612</v>
+        <v>0.01442743041817834</v>
       </c>
       <c r="V8">
         <v>0</v>
       </c>
       <c r="W8">
-        <v>0.007658505086714576</v>
+        <v>0.01371948626917085</v>
       </c>
       <c r="X8">
-        <v>0.02478325568067999</v>
+        <v>0.02863848677037984</v>
       </c>
       <c r="Y8">
-        <v>0.02018285149994988</v>
+        <v>0.02463063673475584</v>
       </c>
       <c r="Z8">
-        <v>0</v>
+        <v>0.006741228664557306</v>
       </c>
       <c r="AA8">
         <v>0</v>
@@ -2363,10 +2363,10 @@
         <v>0</v>
       </c>
       <c r="AD8">
-        <v>0</v>
+        <v>0.004446981228344656</v>
       </c>
       <c r="AE8">
-        <v>0.01160321557743421</v>
+        <v>0.01715609911005561</v>
       </c>
       <c r="AF8">
         <v>0</v>
@@ -2375,13 +2375,13 @@
         <v>0</v>
       </c>
       <c r="AH8">
-        <v>0.00904238017927256</v>
+        <v>0.0149251116057967</v>
       </c>
       <c r="AI8">
-        <v>0.02444696682975859</v>
+        <v>0.02834551353798629</v>
       </c>
       <c r="AJ8">
-        <v>0.05629007326797934</v>
+        <v>0.05608707498760387</v>
       </c>
       <c r="AK8">
         <v>0</v>
@@ -2515,46 +2515,46 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0.1179134946918223</v>
+        <v>0.1135212304626478</v>
       </c>
       <c r="F9">
-        <v>0.0183554702629268</v>
+        <v>0.02202217113585119</v>
       </c>
       <c r="G9">
-        <v>0.09569603518254148</v>
+        <v>0.09310221695377416</v>
       </c>
       <c r="H9">
-        <v>0.01209090311215746</v>
+        <v>0.01626470452607202</v>
       </c>
       <c r="I9">
-        <v>0.07298728256956917</v>
+        <v>0.07223167924984564</v>
       </c>
       <c r="J9">
-        <v>0.004563525169494958</v>
+        <v>0.009346648398483818</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>0.001770524836030253</v>
       </c>
       <c r="M9">
-        <v>0.2620351786288969</v>
+        <v>0.2459766360864747</v>
       </c>
       <c r="N9">
-        <v>0.1249911123441372</v>
+        <v>0.1200259332344877</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>0.0005067763653602818</v>
       </c>
       <c r="P9">
-        <v>0.06165712643233144</v>
+        <v>0.06181867000694534</v>
       </c>
       <c r="Q9">
         <v>0</v>
       </c>
       <c r="R9">
-        <v>0.01252288916095265</v>
+        <v>0.01666172241924335</v>
       </c>
       <c r="S9">
         <v>0</v>
@@ -2563,7 +2563,7 @@
         <v>0</v>
       </c>
       <c r="U9">
-        <v>0.02995617729909208</v>
+        <v>0.03268383088074666</v>
       </c>
       <c r="V9">
         <v>0</v>
@@ -2572,16 +2572,16 @@
         <v>0</v>
       </c>
       <c r="X9">
-        <v>0.08403937075492668</v>
+        <v>0.08238912942383192</v>
       </c>
       <c r="Y9">
-        <v>0.03347887952436204</v>
+        <v>0.03592137945354722</v>
       </c>
       <c r="Z9">
         <v>0</v>
       </c>
       <c r="AA9">
-        <v>0</v>
+        <v>0.001382185452395864</v>
       </c>
       <c r="AB9">
         <v>0</v>
@@ -2605,10 +2605,10 @@
         <v>0</v>
       </c>
       <c r="AI9">
-        <v>0.03039189379499306</v>
+        <v>0.03308427725095944</v>
       </c>
       <c r="AJ9">
-        <v>0.03932066107179593</v>
+        <v>0.04129028386330268</v>
       </c>
       <c r="AK9">
         <v>0</v>
@@ -2742,46 +2742,46 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0.1834483479035048</v>
+        <v>0.1765212686794697</v>
       </c>
       <c r="F10">
-        <v>0.09868925206733722</v>
+        <v>0.09631278544086362</v>
       </c>
       <c r="G10">
-        <v>0.1412585292806602</v>
+        <v>0.1365965700206824</v>
       </c>
       <c r="H10">
-        <v>0.05322447292395576</v>
+        <v>0.05328895490216207</v>
       </c>
       <c r="I10">
-        <v>0.05325716232128996</v>
+        <v>0.05331988924557731</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>0.02399020499160533</v>
+        <v>0.02562423920041337</v>
       </c>
       <c r="L10">
-        <v>0.01682131171582579</v>
+        <v>0.01884023507109657</v>
       </c>
       <c r="M10">
-        <v>0.1854228294438118</v>
+        <v>0.1783897427112924</v>
       </c>
       <c r="N10">
-        <v>0.003908067678128713</v>
+        <v>0.006620287374206564</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>0.0002536955610089835</v>
       </c>
       <c r="P10">
-        <v>0.07212393339297606</v>
+        <v>0.07117372636289376</v>
       </c>
       <c r="Q10">
-        <v>0.02023687831029175</v>
+        <v>0.02207242405612424</v>
       </c>
       <c r="R10">
-        <v>0.0116978624894173</v>
+        <v>0.01399185759200505</v>
       </c>
       <c r="S10">
         <v>0</v>
@@ -2796,13 +2796,13 @@
         <v>0</v>
       </c>
       <c r="W10">
-        <v>0</v>
+        <v>0.0003843947939096492</v>
       </c>
       <c r="X10">
-        <v>0.04340759332505884</v>
+        <v>0.04399913160950318</v>
       </c>
       <c r="Y10">
-        <v>0.02784244972854763</v>
+        <v>0.02926966161043157</v>
       </c>
       <c r="Z10">
         <v>0</v>
@@ -2811,13 +2811,13 @@
         <v>0</v>
       </c>
       <c r="AB10">
-        <v>0</v>
+        <v>0.000453987796996606</v>
       </c>
       <c r="AC10">
         <v>0</v>
       </c>
       <c r="AD10">
-        <v>0.01068838288523369</v>
+        <v>0.01303657571797018</v>
       </c>
       <c r="AE10">
         <v>0</v>
@@ -2826,16 +2826,16 @@
         <v>0</v>
       </c>
       <c r="AG10">
-        <v>0.003720983445460993</v>
+        <v>0.006443247466075156</v>
       </c>
       <c r="AH10">
         <v>0</v>
       </c>
       <c r="AI10">
-        <v>0.01395853284653089</v>
+        <v>0.01613115531170992</v>
       </c>
       <c r="AJ10">
-        <v>0.03630320525036314</v>
+        <v>0.03727616947560757</v>
       </c>
       <c r="AK10">
         <v>0</v>
@@ -2969,55 +2969,55 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0.1698418394585446</v>
+        <v>0.2024147165386041</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.2449806199036375</v>
+        <v>0.3029540848524558</v>
       </c>
       <c r="H11">
-        <v>0.08895842438740055</v>
+        <v>0.09418874573964663</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0.001065897181899224</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>0.04107583087983967</v>
+        <v>0.03011949047675391</v>
       </c>
       <c r="L11">
-        <v>0.01856582489903747</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>0.03782057311391854</v>
+        <v>0.02576379615292029</v>
       </c>
       <c r="N11">
-        <v>0.08341615656435937</v>
+        <v>0.08677291994830406</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11">
-        <v>0.009690195706483782</v>
+        <v>0</v>
       </c>
       <c r="Q11">
         <v>0</v>
       </c>
       <c r="R11">
-        <v>0.07012212624807908</v>
+        <v>0.06898485628228934</v>
       </c>
       <c r="S11">
         <v>0</v>
       </c>
       <c r="T11">
-        <v>0.01159324596035673</v>
+        <v>0</v>
       </c>
       <c r="U11">
-        <v>0.01929577644966685</v>
+        <v>0.0009767109256400837</v>
       </c>
       <c r="V11">
         <v>0</v>
@@ -3026,10 +3026,10 @@
         <v>0</v>
       </c>
       <c r="X11">
-        <v>0.04538870475074969</v>
+        <v>0.03589032694801483</v>
       </c>
       <c r="Y11">
-        <v>0.1042990517826987</v>
+        <v>0.1147152565337431</v>
       </c>
       <c r="Z11">
         <v>0</v>
@@ -3059,10 +3059,10 @@
         <v>0</v>
       </c>
       <c r="AI11">
-        <v>0.007503963675418255</v>
+        <v>0</v>
       </c>
       <c r="AJ11">
-        <v>0.04638176903791005</v>
+        <v>0.03721909560162783</v>
       </c>
       <c r="AK11">
         <v>0</v>
@@ -3553,97 +3553,97 @@
         <v>0</v>
       </c>
       <c r="AR2">
-        <v>0.1883562720413256</v>
+        <v>0.1582799338574765</v>
       </c>
       <c r="AS2">
-        <v>0.2134614359331152</v>
+        <v>0.1880435021263309</v>
       </c>
       <c r="AT2">
-        <v>0.4940755311239409</v>
+        <v>0.4189516727087371</v>
       </c>
       <c r="AU2">
-        <v>0.4940755311239409</v>
+        <v>0.4263876208373285</v>
       </c>
       <c r="AV2">
-        <v>0.4940755311239409</v>
+        <v>0.4361472540549485</v>
       </c>
       <c r="AW2">
-        <v>0.5120718075705244</v>
+        <v>0.4603144843375419</v>
       </c>
       <c r="AX2">
-        <v>0.6039596961801854</v>
+        <v>0.5426514970511633</v>
       </c>
       <c r="AY2">
-        <v>0.6039596961801854</v>
+        <v>0.547693643207342</v>
       </c>
       <c r="AZ2">
-        <v>0.6216893170214501</v>
+        <v>0.5716509538780696</v>
       </c>
       <c r="BA2">
-        <v>0.7082050689098044</v>
+        <v>0.6497588529599777</v>
       </c>
       <c r="BB2">
-        <v>0.71572069730995</v>
+        <v>0.6656753901158334</v>
       </c>
       <c r="BC2">
-        <v>0.71572069730995</v>
+        <v>0.6668760208172696</v>
       </c>
       <c r="BD2">
-        <v>0.71572069730995</v>
+        <v>0.6683869162926217</v>
       </c>
       <c r="BE2">
-        <v>0.7836422601120867</v>
+        <v>0.7318568896078059</v>
       </c>
       <c r="BF2">
-        <v>0.792996967929276</v>
+        <v>0.7492212074579941</v>
       </c>
       <c r="BG2">
-        <v>0.8024060459563362</v>
+        <v>0.766628327233683</v>
       </c>
       <c r="BH2">
-        <v>0.8649030417210005</v>
+        <v>0.8258279121365006</v>
       </c>
       <c r="BI2">
-        <v>0.8649030417210005</v>
+        <v>0.8275206264583589</v>
       </c>
       <c r="BJ2">
-        <v>0.8658160515443823</v>
+        <v>0.8382393762762178</v>
       </c>
       <c r="BK2">
-        <v>0.9512020154970848</v>
+        <v>0.9154578710470516</v>
       </c>
       <c r="BL2">
-        <v>0.9657133554803045</v>
+        <v>0.9368816506195368</v>
       </c>
       <c r="BM2">
-        <v>0.9861660468250008</v>
+        <v>0.9629826473473418</v>
       </c>
       <c r="BN2">
-        <v>0.9861660468250008</v>
+        <v>0.9629920115203411</v>
       </c>
       <c r="BO2">
-        <v>0.9861660468250008</v>
+        <v>0.9632175348944518</v>
       </c>
       <c r="BP2">
-        <v>0.9861660468250008</v>
+        <v>0.9696396549711658</v>
       </c>
       <c r="BQ2">
-        <v>0.9861660468250008</v>
+        <v>0.9708165020994489</v>
       </c>
       <c r="BR2">
-        <v>0.9861660468250008</v>
+        <v>0.9718257763287969</v>
       </c>
       <c r="BS2">
-        <v>0.9861660468250008</v>
+        <v>0.9729617116212412</v>
       </c>
       <c r="BT2">
-        <v>0.9861660468250008</v>
+        <v>0.9732905842694807</v>
       </c>
       <c r="BU2">
-        <v>0.9861660468250008</v>
+        <v>0.9745095630543226</v>
       </c>
       <c r="BV2">
-        <v>0.9861660468250008</v>
+        <v>0.9791094804566622</v>
       </c>
       <c r="BW2">
         <v>1</v>
@@ -3780,97 +3780,97 @@
         <v>0</v>
       </c>
       <c r="AR3">
-        <v>0.2810718858277978</v>
+        <v>0.2359324336513552</v>
       </c>
       <c r="AS3">
-        <v>0.3767729848928042</v>
+        <v>0.3228593100309918</v>
       </c>
       <c r="AT3">
-        <v>0.6849581931659249</v>
+        <v>0.5805860932182474</v>
       </c>
       <c r="AU3">
-        <v>0.6849581931659249</v>
+        <v>0.5874809660678627</v>
       </c>
       <c r="AV3">
-        <v>0.6849581931659249</v>
+        <v>0.5889114921401726</v>
       </c>
       <c r="AW3">
-        <v>0.6892927023306435</v>
+        <v>0.6023956762711639</v>
       </c>
       <c r="AX3">
-        <v>0.8040076679140001</v>
+        <v>0.7046063620683128</v>
       </c>
       <c r="AY3">
-        <v>0.811943846677722</v>
+        <v>0.7209856560225948</v>
       </c>
       <c r="AZ3">
-        <v>0.83850035566433</v>
+        <v>0.7523324253266738</v>
       </c>
       <c r="BA3">
-        <v>0.8503451259269302</v>
+        <v>0.7718535404093471</v>
       </c>
       <c r="BB3">
-        <v>0.8503451259269302</v>
+        <v>0.7726349793216989</v>
       </c>
       <c r="BC3">
-        <v>0.8503451259269302</v>
+        <v>0.7738724442421642</v>
       </c>
       <c r="BD3">
-        <v>0.8524707944528582</v>
+        <v>0.7855811084217372</v>
       </c>
       <c r="BE3">
-        <v>0.8603999959865412</v>
+        <v>0.8019547939084266</v>
       </c>
       <c r="BF3">
-        <v>0.8858791532281153</v>
+        <v>0.8324355616167318</v>
       </c>
       <c r="BG3">
-        <v>0.8858791532281153</v>
+        <v>0.8335222326116345</v>
       </c>
       <c r="BH3">
-        <v>0.9006076888876728</v>
+        <v>0.855361388619302</v>
       </c>
       <c r="BI3">
-        <v>0.9006076888876728</v>
+        <v>0.8583731793117582</v>
       </c>
       <c r="BJ3">
-        <v>0.9006076888876728</v>
+        <v>0.8586307178578062</v>
       </c>
       <c r="BK3">
-        <v>0.9641103781698777</v>
+        <v>0.9196757275380857</v>
       </c>
       <c r="BL3">
-        <v>0.9641103781698777</v>
+        <v>0.9266725170837539</v>
       </c>
       <c r="BM3">
-        <v>0.9694775291068046</v>
+        <v>0.9409867638444455</v>
       </c>
       <c r="BN3">
-        <v>0.9694775291068046</v>
+        <v>0.9409892666723595</v>
       </c>
       <c r="BO3">
-        <v>0.9694775291068046</v>
+        <v>0.9410135033752115</v>
       </c>
       <c r="BP3">
-        <v>0.9694775291068046</v>
+        <v>0.9437397219733978</v>
       </c>
       <c r="BQ3">
-        <v>0.9694775291068046</v>
+        <v>0.946157701313544</v>
       </c>
       <c r="BR3">
-        <v>0.9694775291068046</v>
+        <v>0.9463226398556441</v>
       </c>
       <c r="BS3">
-        <v>0.9694775291068046</v>
+        <v>0.9468936062934651</v>
       </c>
       <c r="BT3">
-        <v>0.9694775291068046</v>
+        <v>0.9492567774731874</v>
       </c>
       <c r="BU3">
-        <v>0.9694775291068046</v>
+        <v>0.9554652938352673</v>
       </c>
       <c r="BV3">
-        <v>0.97839331683122</v>
+        <v>0.972632021352548</v>
       </c>
       <c r="BW3">
         <v>1</v>
@@ -4007,100 +4007,100 @@
         <v>0</v>
       </c>
       <c r="AR4">
-        <v>0.2847639121176406</v>
+        <v>0.2412224171542024</v>
       </c>
       <c r="AS4">
-        <v>0.4255236696840377</v>
+        <v>0.3655164340487879</v>
       </c>
       <c r="AT4">
-        <v>0.6964415132398433</v>
+        <v>0.5954961294088478</v>
       </c>
       <c r="AU4">
-        <v>0.6964415132398433</v>
+        <v>0.5965752760274327</v>
       </c>
       <c r="AV4">
-        <v>0.6964415132398433</v>
+        <v>0.5986029487014615</v>
       </c>
       <c r="AW4">
-        <v>0.6964415132398433</v>
+        <v>0.5999855423510049</v>
       </c>
       <c r="AX4">
-        <v>0.8202418225548799</v>
+        <v>0.7105088374251191</v>
       </c>
       <c r="AY4">
-        <v>0.8392008418937358</v>
+        <v>0.7359031696837394</v>
       </c>
       <c r="AZ4">
-        <v>0.8709771755134711</v>
+        <v>0.771704896500929</v>
       </c>
       <c r="BA4">
-        <v>0.8750840000031576</v>
+        <v>0.7850395531934564</v>
       </c>
       <c r="BB4">
-        <v>0.8750840000031576</v>
+        <v>0.7850806844456436</v>
       </c>
       <c r="BC4">
-        <v>0.8750840000031576</v>
+        <v>0.7857467834285954</v>
       </c>
       <c r="BD4">
-        <v>0.8781238267714191</v>
+        <v>0.798215060001496</v>
       </c>
       <c r="BE4">
-        <v>0.8781238267714191</v>
+        <v>0.8038585972335438</v>
       </c>
       <c r="BF4">
-        <v>0.8941082534080622</v>
+        <v>0.8268376216340155</v>
       </c>
       <c r="BG4">
-        <v>0.8941082534080622</v>
+        <v>0.8319026120927445</v>
       </c>
       <c r="BH4">
-        <v>0.8989578481453649</v>
+        <v>0.8458403828904507</v>
       </c>
       <c r="BI4">
-        <v>0.8989578481453649</v>
+        <v>0.8473598883346174</v>
       </c>
       <c r="BJ4">
-        <v>0.8989578481453649</v>
+        <v>0.8518501188988894</v>
       </c>
       <c r="BK4">
-        <v>0.9673247233641075</v>
+        <v>0.9173626100140798</v>
       </c>
       <c r="BL4">
-        <v>0.9673247233641075</v>
+        <v>0.9241710052669215</v>
       </c>
       <c r="BM4">
-        <v>0.9673247233641075</v>
+        <v>0.9320706250501288</v>
       </c>
       <c r="BN4">
-        <v>0.9673247233641075</v>
+        <v>0.9329340483489615</v>
       </c>
       <c r="BO4">
-        <v>0.9673247233641075</v>
+        <v>0.9347383635320866</v>
       </c>
       <c r="BP4">
-        <v>0.9673247233641075</v>
+        <v>0.9351781811192305</v>
       </c>
       <c r="BQ4">
-        <v>0.9673247233641075</v>
+        <v>0.9373357033034668</v>
       </c>
       <c r="BR4">
-        <v>0.9673247233641075</v>
+        <v>0.9384524380066318</v>
       </c>
       <c r="BS4">
-        <v>0.9673247233641075</v>
+        <v>0.9397656226898902</v>
       </c>
       <c r="BT4">
-        <v>0.9673247233641075</v>
+        <v>0.9434683500140563</v>
       </c>
       <c r="BU4">
-        <v>0.9681741271317466</v>
+        <v>0.9541580483358445</v>
       </c>
       <c r="BV4">
-        <v>0.983144177339568</v>
+        <v>0.9763134200198179</v>
       </c>
       <c r="BW4">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:75">
@@ -4234,100 +4234,100 @@
         <v>0</v>
       </c>
       <c r="AR5">
-        <v>0.2016516135182773</v>
+        <v>0.1696070221949173</v>
       </c>
       <c r="AS5">
-        <v>0.2419981015036753</v>
+        <v>0.2115412214359698</v>
       </c>
       <c r="AT5">
-        <v>0.5653763890616422</v>
+        <v>0.477494767351637</v>
       </c>
       <c r="AU5">
-        <v>0.5727846968029785</v>
+        <v>0.4933584344826272</v>
       </c>
       <c r="AV5">
-        <v>0.5727846968029785</v>
+        <v>0.496527453960981</v>
       </c>
       <c r="AW5">
-        <v>0.6045108543950505</v>
+        <v>0.5316386715238313</v>
       </c>
       <c r="AX5">
-        <v>0.7120541829639587</v>
+        <v>0.6267590934750161</v>
       </c>
       <c r="AY5">
-        <v>0.7225087441031007</v>
+        <v>0.6450338666973088</v>
       </c>
       <c r="AZ5">
-        <v>0.7557419011831535</v>
+        <v>0.6813378726367525</v>
       </c>
       <c r="BA5">
-        <v>0.7812147983968069</v>
+        <v>0.7114996417394822</v>
       </c>
       <c r="BB5">
-        <v>0.7812147983968069</v>
+        <v>0.7130729478795759</v>
       </c>
       <c r="BC5">
-        <v>0.7812147983968069</v>
+        <v>0.7148611609161984</v>
       </c>
       <c r="BD5">
-        <v>0.7812147983968069</v>
+        <v>0.7187512993792402</v>
       </c>
       <c r="BE5">
-        <v>0.8058925341342225</v>
+        <v>0.7482836990800985</v>
       </c>
       <c r="BF5">
-        <v>0.8173939251947918</v>
+        <v>0.7673870369917009</v>
       </c>
       <c r="BG5">
-        <v>0.8173939251947918</v>
+        <v>0.7718261133335999</v>
       </c>
       <c r="BH5">
-        <v>0.8525674579445498</v>
+        <v>0.8096659244033756</v>
       </c>
       <c r="BI5">
-        <v>0.8525674579445498</v>
+        <v>0.8099757788861701</v>
       </c>
       <c r="BJ5">
-        <v>0.8525674579445498</v>
+        <v>0.8110590299518452</v>
       </c>
       <c r="BK5">
-        <v>0.9447972003991242</v>
+        <v>0.8940587659526906</v>
       </c>
       <c r="BL5">
-        <v>0.9561015682384308</v>
+        <v>0.9130061602092915</v>
       </c>
       <c r="BM5">
-        <v>0.9779703980941741</v>
+        <v>0.9403153141072648</v>
       </c>
       <c r="BN5">
-        <v>0.9779703980941741</v>
+        <v>0.9404279923292063</v>
       </c>
       <c r="BO5">
-        <v>0.9779703980941741</v>
+        <v>0.9412251164497351</v>
       </c>
       <c r="BP5">
-        <v>0.9779703980941741</v>
+        <v>0.9480161241431674</v>
       </c>
       <c r="BQ5">
-        <v>0.9779703980941741</v>
+        <v>0.9532722571533383</v>
       </c>
       <c r="BR5">
-        <v>0.9779703980941741</v>
+        <v>0.9534404884060891</v>
       </c>
       <c r="BS5">
-        <v>0.9779703980941741</v>
+        <v>0.9538701182392346</v>
       </c>
       <c r="BT5">
-        <v>0.9779703980941741</v>
+        <v>0.9571514960375498</v>
       </c>
       <c r="BU5">
-        <v>0.9779703980941741</v>
+        <v>0.9625635952076838</v>
       </c>
       <c r="BV5">
-        <v>0.9812755681179308</v>
+        <v>0.9751796335132334</v>
       </c>
       <c r="BW5">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:75">
@@ -4458,97 +4458,97 @@
         <v>0</v>
       </c>
       <c r="AQ6">
-        <v>0.005630125271338065</v>
+        <v>0.01453263636904105</v>
       </c>
       <c r="AR6">
-        <v>0.2268442450969968</v>
+        <v>0.2026251505750147</v>
       </c>
       <c r="AS6">
-        <v>0.4533727227472666</v>
+        <v>0.394996086733082</v>
       </c>
       <c r="AT6">
-        <v>0.6341180055275609</v>
+        <v>0.5505084159938954</v>
       </c>
       <c r="AU6">
-        <v>0.6341180055275609</v>
+        <v>0.5517532887261876</v>
       </c>
       <c r="AV6">
-        <v>0.6341180055275609</v>
+        <v>0.5544346403594977</v>
       </c>
       <c r="AW6">
-        <v>0.6392244382899546</v>
+        <v>0.5685456683987349</v>
       </c>
       <c r="AX6">
-        <v>0.8365332920813429</v>
+        <v>0.7373928065222001</v>
       </c>
       <c r="AY6">
-        <v>0.8520881531606741</v>
+        <v>0.7599155348178712</v>
       </c>
       <c r="AZ6">
-        <v>0.8551850669519371</v>
+        <v>0.7724087624825422</v>
       </c>
       <c r="BA6">
-        <v>0.8551850669519371</v>
+        <v>0.7809450280965397</v>
       </c>
       <c r="BB6">
-        <v>0.8551850669519371</v>
+        <v>0.7811857013929623</v>
       </c>
       <c r="BC6">
-        <v>0.8551850669519371</v>
+        <v>0.7842662670313089</v>
       </c>
       <c r="BD6">
-        <v>0.8651024746499404</v>
+        <v>0.8022504593276011</v>
       </c>
       <c r="BE6">
-        <v>0.8651024746499404</v>
+        <v>0.8023683709817937</v>
       </c>
       <c r="BF6">
-        <v>0.8651024746499404</v>
+        <v>0.8112667961413697</v>
       </c>
       <c r="BG6">
-        <v>0.8786506040107827</v>
+        <v>0.8321739679917096</v>
       </c>
       <c r="BH6">
-        <v>0.8786506040107827</v>
+        <v>0.8375811477110514</v>
       </c>
       <c r="BI6">
-        <v>0.8786506040107827</v>
+        <v>0.839300128894762</v>
       </c>
       <c r="BJ6">
-        <v>0.8973610941437127</v>
+        <v>0.8643633546618411</v>
       </c>
       <c r="BK6">
-        <v>0.9798226879535833</v>
+        <v>0.9407505842772275</v>
       </c>
       <c r="BL6">
-        <v>0.9798226879535833</v>
+        <v>0.9407526980353805</v>
       </c>
       <c r="BM6">
-        <v>0.9798226879535833</v>
+        <v>0.9467734983667366</v>
       </c>
       <c r="BN6">
-        <v>0.9798226879535833</v>
+        <v>0.9479725603035423</v>
       </c>
       <c r="BO6">
-        <v>0.9798226879535833</v>
+        <v>0.9481465834681007</v>
       </c>
       <c r="BP6">
-        <v>0.9798226879535833</v>
+        <v>0.9502732260046871</v>
       </c>
       <c r="BQ6">
-        <v>0.9798226879535833</v>
+        <v>0.9538209919495072</v>
       </c>
       <c r="BR6">
-        <v>0.9798226879535833</v>
+        <v>0.9553890318524557</v>
       </c>
       <c r="BS6">
-        <v>0.9798226879535833</v>
+        <v>0.9554175661798253</v>
       </c>
       <c r="BT6">
-        <v>0.9798226879535833</v>
+        <v>0.9637558821512078</v>
       </c>
       <c r="BU6">
-        <v>0.981876572591043</v>
+        <v>0.9754093999251298</v>
       </c>
       <c r="BV6">
         <v>0.9999999999999999</v>
@@ -4568,220 +4568,220 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.002056664043484111</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0.1313908317085751</v>
+        <v>0.1405024519496363</v>
       </c>
       <c r="F7">
-        <v>0.1521164865947558</v>
+        <v>0.1533200956914033</v>
       </c>
       <c r="G7">
-        <v>0.4276195501204607</v>
+        <v>0.46566494706613</v>
       </c>
       <c r="H7">
-        <v>0.4937478051014808</v>
+        <v>0.5318598274251528</v>
       </c>
       <c r="I7">
-        <v>0.5141632497742766</v>
+        <v>0.5443127747855155</v>
       </c>
       <c r="J7">
-        <v>0.5141632497742766</v>
+        <v>0.5443127747855155</v>
       </c>
       <c r="K7">
-        <v>0.5141632497742766</v>
+        <v>0.5443127747855155</v>
       </c>
       <c r="L7">
-        <v>0.5141632497742766</v>
+        <v>0.5443127747855155</v>
       </c>
       <c r="M7">
-        <v>0.7547315322035367</v>
+        <v>0.8155868048226571</v>
       </c>
       <c r="N7">
-        <v>0.8021363251285796</v>
+        <v>0.8597695831794049</v>
       </c>
       <c r="O7">
-        <v>0.8021363251285796</v>
+        <v>0.8597695831794049</v>
       </c>
       <c r="P7">
-        <v>0.8608872393010963</v>
+        <v>0.9172913464676199</v>
       </c>
       <c r="Q7">
-        <v>0.8707102250000635</v>
+        <v>0.9172913464676199</v>
       </c>
       <c r="R7">
-        <v>0.8905487418086843</v>
+        <v>0.9290660327800948</v>
       </c>
       <c r="S7">
-        <v>0.9039457816448612</v>
+        <v>0.9332678435346823</v>
       </c>
       <c r="T7">
-        <v>0.9039457816448612</v>
+        <v>0.9332678435346823</v>
       </c>
       <c r="U7">
-        <v>0.9039457816448612</v>
+        <v>0.9332678435346823</v>
       </c>
       <c r="V7">
-        <v>0.9039457816448612</v>
+        <v>0.9332678435346823</v>
       </c>
       <c r="W7">
-        <v>0.9297602136609067</v>
+        <v>0.9520680711017343</v>
       </c>
       <c r="X7">
-        <v>0.9555036705530647</v>
+        <v>0.9707848572805451</v>
       </c>
       <c r="Y7">
-        <v>0.9658785843539063</v>
+        <v>0.9714337275396916</v>
       </c>
       <c r="Z7">
-        <v>0.9658785843539063</v>
+        <v>0.9714337275396916</v>
       </c>
       <c r="AA7">
-        <v>0.9658785843539063</v>
+        <v>0.9714337275396916</v>
       </c>
       <c r="AB7">
-        <v>0.9658785843539063</v>
+        <v>0.9714337275396916</v>
       </c>
       <c r="AC7">
-        <v>0.9658785843539063</v>
+        <v>0.9714337275396916</v>
       </c>
       <c r="AD7">
-        <v>0.9658785843539063</v>
+        <v>0.9714337275396916</v>
       </c>
       <c r="AE7">
-        <v>0.9658785843539063</v>
+        <v>0.9714337275396916</v>
       </c>
       <c r="AF7">
-        <v>0.9658785843539063</v>
+        <v>0.9714337275396916</v>
       </c>
       <c r="AG7">
-        <v>0.9658785843539063</v>
+        <v>0.9714337275396916</v>
       </c>
       <c r="AH7">
-        <v>0.9658785843539063</v>
+        <v>0.9714337275396916</v>
       </c>
       <c r="AI7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AJ7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AK7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AL7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AM7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AN7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AO7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AP7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AQ7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AR7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AS7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AT7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AU7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AV7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AW7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AX7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AY7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AZ7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BA7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BB7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BC7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BD7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BE7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BF7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BG7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BH7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BI7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BJ7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BK7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BL7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BM7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BN7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BO7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BP7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BQ7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BR7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BS7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BT7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BU7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BV7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BW7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:75">
@@ -4798,97 +4798,97 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0.1714552967088327</v>
+        <v>0.1564184647388446</v>
       </c>
       <c r="F8">
-        <v>0.1714552967088327</v>
+        <v>0.1570442367810624</v>
       </c>
       <c r="G8">
-        <v>0.2983263879009753</v>
+        <v>0.2746211557233864</v>
       </c>
       <c r="H8">
-        <v>0.4361606168251749</v>
+        <v>0.4017491076236454</v>
       </c>
       <c r="I8">
-        <v>0.5043991094398227</v>
+        <v>0.4682455881814779</v>
       </c>
       <c r="J8">
-        <v>0.5043991094398227</v>
+        <v>0.4688781531501079</v>
       </c>
       <c r="K8">
-        <v>0.5043991094398227</v>
+        <v>0.4715363382407158</v>
       </c>
       <c r="L8">
-        <v>0.5043991094398227</v>
+        <v>0.4724774727653378</v>
       </c>
       <c r="M8">
-        <v>0.6582496554550267</v>
+        <v>0.6135587632206365</v>
       </c>
       <c r="N8">
-        <v>0.6902915281852854</v>
+        <v>0.6485209223158507</v>
       </c>
       <c r="O8">
-        <v>0.6902915281852854</v>
+        <v>0.6485209223158507</v>
       </c>
       <c r="P8">
-        <v>0.7709127467378929</v>
+        <v>0.7258051742611309</v>
       </c>
       <c r="Q8">
-        <v>0.7709127467378929</v>
+        <v>0.7258051742611309</v>
       </c>
       <c r="R8">
-        <v>0.8375216342451512</v>
+        <v>0.790881950673171</v>
       </c>
       <c r="S8">
-        <v>0.8375216342451512</v>
+        <v>0.790881950673171</v>
       </c>
       <c r="T8">
-        <v>0.8375216342451512</v>
+        <v>0.790881950673171</v>
       </c>
       <c r="U8">
-        <v>0.8459927518782109</v>
+        <v>0.8053093810913493</v>
       </c>
       <c r="V8">
-        <v>0.8459927518782109</v>
+        <v>0.8053093810913493</v>
       </c>
       <c r="W8">
-        <v>0.8536512569649255</v>
+        <v>0.8190288673605202</v>
       </c>
       <c r="X8">
-        <v>0.8784345126456055</v>
+        <v>0.8476673541309</v>
       </c>
       <c r="Y8">
-        <v>0.8986173641455554</v>
+        <v>0.8722979908656558</v>
       </c>
       <c r="Z8">
-        <v>0.8986173641455554</v>
+        <v>0.8790392195302131</v>
       </c>
       <c r="AA8">
-        <v>0.8986173641455554</v>
+        <v>0.8790392195302131</v>
       </c>
       <c r="AB8">
-        <v>0.8986173641455554</v>
+        <v>0.8790392195302131</v>
       </c>
       <c r="AC8">
-        <v>0.8986173641455554</v>
+        <v>0.8790392195302131</v>
       </c>
       <c r="AD8">
-        <v>0.8986173641455554</v>
+        <v>0.8834862007585578</v>
       </c>
       <c r="AE8">
-        <v>0.9102205797229895</v>
+        <v>0.9006422998686134</v>
       </c>
       <c r="AF8">
-        <v>0.9102205797229895</v>
+        <v>0.9006422998686134</v>
       </c>
       <c r="AG8">
-        <v>0.9102205797229895</v>
+        <v>0.9006422998686134</v>
       </c>
       <c r="AH8">
-        <v>0.9192629599022621</v>
+        <v>0.9155674114744101</v>
       </c>
       <c r="AI8">
-        <v>0.9437099267320207</v>
+        <v>0.9439129250123964</v>
       </c>
       <c r="AJ8">
         <v>1</v>
@@ -5025,217 +5025,217 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0.1179134946918223</v>
+        <v>0.1135212304626478</v>
       </c>
       <c r="F9">
-        <v>0.1362689649547491</v>
+        <v>0.135543401598499</v>
       </c>
       <c r="G9">
-        <v>0.2319650001372906</v>
+        <v>0.2286456185522732</v>
       </c>
       <c r="H9">
-        <v>0.2440559032494481</v>
+        <v>0.2449103230783452</v>
       </c>
       <c r="I9">
-        <v>0.3170431858190172</v>
+        <v>0.3171420023281908</v>
       </c>
       <c r="J9">
-        <v>0.3216067109885122</v>
+        <v>0.3264886507266746</v>
       </c>
       <c r="K9">
-        <v>0.3216067109885122</v>
+        <v>0.3264886507266746</v>
       </c>
       <c r="L9">
-        <v>0.3216067109885122</v>
+        <v>0.3282591755627048</v>
       </c>
       <c r="M9">
-        <v>0.5836418896174091</v>
+        <v>0.5742358116491796</v>
       </c>
       <c r="N9">
-        <v>0.7086330019615463</v>
+        <v>0.6942617448836672</v>
       </c>
       <c r="O9">
-        <v>0.7086330019615463</v>
+        <v>0.6947685212490274</v>
       </c>
       <c r="P9">
-        <v>0.7702901283938778</v>
+        <v>0.7565871912559727</v>
       </c>
       <c r="Q9">
-        <v>0.7702901283938778</v>
+        <v>0.7565871912559727</v>
       </c>
       <c r="R9">
-        <v>0.7828130175548305</v>
+        <v>0.7732489136752161</v>
       </c>
       <c r="S9">
-        <v>0.7828130175548305</v>
+        <v>0.7732489136752161</v>
       </c>
       <c r="T9">
-        <v>0.7828130175548305</v>
+        <v>0.7732489136752161</v>
       </c>
       <c r="U9">
-        <v>0.8127691948539225</v>
+        <v>0.8059327445559628</v>
       </c>
       <c r="V9">
-        <v>0.8127691948539225</v>
+        <v>0.8059327445559628</v>
       </c>
       <c r="W9">
-        <v>0.8127691948539225</v>
+        <v>0.8059327445559628</v>
       </c>
       <c r="X9">
-        <v>0.8968085656088491</v>
+        <v>0.8883218739797947</v>
       </c>
       <c r="Y9">
-        <v>0.9302874451332112</v>
+        <v>0.9242432534333419</v>
       </c>
       <c r="Z9">
-        <v>0.9302874451332112</v>
+        <v>0.9242432534333419</v>
       </c>
       <c r="AA9">
-        <v>0.9302874451332112</v>
+        <v>0.9256254388857378</v>
       </c>
       <c r="AB9">
-        <v>0.9302874451332112</v>
+        <v>0.9256254388857378</v>
       </c>
       <c r="AC9">
-        <v>0.9302874451332112</v>
+        <v>0.9256254388857378</v>
       </c>
       <c r="AD9">
-        <v>0.9302874451332112</v>
+        <v>0.9256254388857378</v>
       </c>
       <c r="AE9">
-        <v>0.9302874451332112</v>
+        <v>0.9256254388857378</v>
       </c>
       <c r="AF9">
-        <v>0.9302874451332112</v>
+        <v>0.9256254388857378</v>
       </c>
       <c r="AG9">
-        <v>0.9302874451332112</v>
+        <v>0.9256254388857378</v>
       </c>
       <c r="AH9">
-        <v>0.9302874451332112</v>
+        <v>0.9256254388857378</v>
       </c>
       <c r="AI9">
-        <v>0.9606793389282042</v>
+        <v>0.9587097161366972</v>
       </c>
       <c r="AJ9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AK9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AL9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AM9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AN9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AO9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AP9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AQ9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AR9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AS9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AT9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AU9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AV9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AW9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AX9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AY9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AZ9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BA9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BB9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BC9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BD9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BE9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BF9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BG9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BH9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BI9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BJ9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BK9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BL9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BM9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BN9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BO9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BP9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BQ9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BR9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BS9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BT9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BU9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BV9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BW9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:75">
@@ -5252,217 +5252,217 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0.1834483479035048</v>
+        <v>0.1765212686794697</v>
       </c>
       <c r="F10">
-        <v>0.282137599970842</v>
+        <v>0.2728340541203333</v>
       </c>
       <c r="G10">
-        <v>0.4233961292515022</v>
+        <v>0.4094306241410157</v>
       </c>
       <c r="H10">
-        <v>0.4766206021754579</v>
+        <v>0.4627195790431778</v>
       </c>
       <c r="I10">
-        <v>0.5298777644967478</v>
+        <v>0.5160394682887551</v>
       </c>
       <c r="J10">
-        <v>0.5298777644967478</v>
+        <v>0.5160394682887551</v>
       </c>
       <c r="K10">
-        <v>0.5538679694883532</v>
+        <v>0.5416637074891685</v>
       </c>
       <c r="L10">
-        <v>0.5706892812041789</v>
+        <v>0.560503942560265</v>
       </c>
       <c r="M10">
-        <v>0.7561121106479907</v>
+        <v>0.7388936852715574</v>
       </c>
       <c r="N10">
-        <v>0.7600201783261193</v>
+        <v>0.745513972645764</v>
       </c>
       <c r="O10">
-        <v>0.7600201783261193</v>
+        <v>0.745767668206773</v>
       </c>
       <c r="P10">
-        <v>0.8321441117190954</v>
+        <v>0.8169413945696667</v>
       </c>
       <c r="Q10">
-        <v>0.8523809900293872</v>
+        <v>0.8390138186257909</v>
       </c>
       <c r="R10">
-        <v>0.8640788525188045</v>
+        <v>0.853005676217796</v>
       </c>
       <c r="S10">
-        <v>0.8640788525188045</v>
+        <v>0.853005676217796</v>
       </c>
       <c r="T10">
-        <v>0.8640788525188045</v>
+        <v>0.853005676217796</v>
       </c>
       <c r="U10">
-        <v>0.8640788525188045</v>
+        <v>0.853005676217796</v>
       </c>
       <c r="V10">
-        <v>0.8640788525188045</v>
+        <v>0.853005676217796</v>
       </c>
       <c r="W10">
-        <v>0.8640788525188045</v>
+        <v>0.8533900710117056</v>
       </c>
       <c r="X10">
-        <v>0.9074864458438633</v>
+        <v>0.8973892026212088</v>
       </c>
       <c r="Y10">
-        <v>0.9353288955724109</v>
+        <v>0.9266588642316403</v>
       </c>
       <c r="Z10">
-        <v>0.9353288955724109</v>
+        <v>0.9266588642316403</v>
       </c>
       <c r="AA10">
-        <v>0.9353288955724109</v>
+        <v>0.9266588642316403</v>
       </c>
       <c r="AB10">
-        <v>0.9353288955724109</v>
+        <v>0.9271128520286369</v>
       </c>
       <c r="AC10">
-        <v>0.9353288955724109</v>
+        <v>0.9271128520286369</v>
       </c>
       <c r="AD10">
-        <v>0.9460172784576446</v>
+        <v>0.9401494277466071</v>
       </c>
       <c r="AE10">
-        <v>0.9460172784576446</v>
+        <v>0.9401494277466071</v>
       </c>
       <c r="AF10">
-        <v>0.9460172784576446</v>
+        <v>0.9401494277466071</v>
       </c>
       <c r="AG10">
-        <v>0.9497382619031056</v>
+        <v>0.9465926752126823</v>
       </c>
       <c r="AH10">
-        <v>0.9497382619031056</v>
+        <v>0.9465926752126823</v>
       </c>
       <c r="AI10">
-        <v>0.9636967947496365</v>
+        <v>0.9627238305243923</v>
       </c>
       <c r="AJ10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AK10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AL10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AM10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AN10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AO10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AP10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AQ10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AR10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AS10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AT10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AU10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AV10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AW10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AX10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AY10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AZ10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BA10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BB10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BC10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BD10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BE10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BF10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BG10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BH10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BI10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BJ10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BK10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BL10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BM10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BN10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BO10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BP10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BQ10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BR10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BS10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BT10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BU10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BV10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="BW10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:75">
@@ -5479,97 +5479,97 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0.1698418394585446</v>
+        <v>0.2024147165386041</v>
       </c>
       <c r="F11">
-        <v>0.1698418394585446</v>
+        <v>0.2024147165386041</v>
       </c>
       <c r="G11">
-        <v>0.4148224593621821</v>
+        <v>0.50536880139106</v>
       </c>
       <c r="H11">
-        <v>0.5037808837495826</v>
+        <v>0.5995575471307066</v>
       </c>
       <c r="I11">
-        <v>0.5037808837495826</v>
+        <v>0.5995575471307066</v>
       </c>
       <c r="J11">
-        <v>0.5048467809314818</v>
+        <v>0.5995575471307066</v>
       </c>
       <c r="K11">
-        <v>0.5459226118113215</v>
+        <v>0.6296770376074605</v>
       </c>
       <c r="L11">
-        <v>0.564488436710359</v>
+        <v>0.6296770376074605</v>
       </c>
       <c r="M11">
-        <v>0.6023090098242775</v>
+        <v>0.6554408337603808</v>
       </c>
       <c r="N11">
-        <v>0.6857251663886369</v>
+        <v>0.7422137537086848</v>
       </c>
       <c r="O11">
-        <v>0.6857251663886369</v>
+        <v>0.7422137537086848</v>
       </c>
       <c r="P11">
-        <v>0.6954153620951207</v>
+        <v>0.7422137537086848</v>
       </c>
       <c r="Q11">
-        <v>0.6954153620951207</v>
+        <v>0.7422137537086848</v>
       </c>
       <c r="R11">
-        <v>0.7655374883431998</v>
+        <v>0.8111986099909742</v>
       </c>
       <c r="S11">
-        <v>0.7655374883431998</v>
+        <v>0.8111986099909742</v>
       </c>
       <c r="T11">
-        <v>0.7771307343035565</v>
+        <v>0.8111986099909742</v>
       </c>
       <c r="U11">
-        <v>0.7964265107532233</v>
+        <v>0.8121753209166143</v>
       </c>
       <c r="V11">
-        <v>0.7964265107532233</v>
+        <v>0.8121753209166143</v>
       </c>
       <c r="W11">
-        <v>0.7964265107532233</v>
+        <v>0.8121753209166143</v>
       </c>
       <c r="X11">
-        <v>0.8418152155039731</v>
+        <v>0.8480656478646291</v>
       </c>
       <c r="Y11">
-        <v>0.9461142672866718</v>
+        <v>0.9627809043983722</v>
       </c>
       <c r="Z11">
-        <v>0.9461142672866718</v>
+        <v>0.9627809043983722</v>
       </c>
       <c r="AA11">
-        <v>0.9461142672866718</v>
+        <v>0.9627809043983722</v>
       </c>
       <c r="AB11">
-        <v>0.9461142672866718</v>
+        <v>0.9627809043983722</v>
       </c>
       <c r="AC11">
-        <v>0.9461142672866718</v>
+        <v>0.9627809043983722</v>
       </c>
       <c r="AD11">
-        <v>0.9461142672866718</v>
+        <v>0.9627809043983722</v>
       </c>
       <c r="AE11">
-        <v>0.9461142672866718</v>
+        <v>0.9627809043983722</v>
       </c>
       <c r="AF11">
-        <v>0.9461142672866718</v>
+        <v>0.9627809043983722</v>
       </c>
       <c r="AG11">
-        <v>0.9461142672866718</v>
+        <v>0.9627809043983722</v>
       </c>
       <c r="AH11">
-        <v>0.9461142672866718</v>
+        <v>0.9627809043983722</v>
       </c>
       <c r="AI11">
-        <v>0.9536182309620901</v>
+        <v>0.9627809043983722</v>
       </c>
       <c r="AJ11">
         <v>1</v>
@@ -5757,16 +5757,16 @@
         <v>41</v>
       </c>
       <c r="D2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.5120718075705244</v>
+        <v>0.5426514970511633</v>
       </c>
       <c r="G2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -5804,7 +5804,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.6849581931659249</v>
+        <v>0.5805860932182474</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -5845,7 +5845,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.6964415132398433</v>
+        <v>0.5954961294088478</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -5880,16 +5880,16 @@
         <v>41</v>
       </c>
       <c r="D5">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.5653763890616422</v>
+        <v>0.5316386715238313</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -5927,7 +5927,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.6341180055275609</v>
+        <v>0.5505084159938954</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -5962,16 +5962,16 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.5141632497742766</v>
+        <v>0.5318598274251528</v>
       </c>
       <c r="G7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H7">
         <v>10</v>
@@ -6003,16 +6003,16 @@
         <v>2</v>
       </c>
       <c r="D8">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.5043991094398227</v>
+        <v>0.6135587632206365</v>
       </c>
       <c r="G8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H8">
         <v>10</v>
@@ -6050,7 +6050,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.5836418896174091</v>
+        <v>0.5742358116491796</v>
       </c>
       <c r="G9">
         <v>10</v>
@@ -6091,7 +6091,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0.5298777644967478</v>
+        <v>0.5160394682887551</v>
       </c>
       <c r="G10">
         <v>6</v>
@@ -6126,16 +6126,16 @@
         <v>2</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0.5037808837495826</v>
+        <v>0.50536880139106</v>
       </c>
       <c r="G11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H11">
         <v>10</v>
@@ -6221,16 +6221,16 @@
         <v>41</v>
       </c>
       <c r="D2">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.7082050689098044</v>
+        <v>0.7318568896078059</v>
       </c>
       <c r="G2">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -6268,7 +6268,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.8040076679140001</v>
+        <v>0.7046063620683128</v>
       </c>
       <c r="G3">
         <v>8</v>
@@ -6309,7 +6309,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.8202418225548799</v>
+        <v>0.7105088374251191</v>
       </c>
       <c r="G4">
         <v>8</v>
@@ -6344,16 +6344,16 @@
         <v>41</v>
       </c>
       <c r="D5">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.7120541829639587</v>
+        <v>0.7114996417394822</v>
       </c>
       <c r="G5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -6391,7 +6391,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.8365332920813429</v>
+        <v>0.7373928065222001</v>
       </c>
       <c r="G6">
         <v>8</v>
@@ -6432,7 +6432,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.7547315322035367</v>
+        <v>0.8155868048226571</v>
       </c>
       <c r="G7">
         <v>10</v>
@@ -6473,7 +6473,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.7709127467378929</v>
+        <v>0.7258051742611309</v>
       </c>
       <c r="G8">
         <v>13</v>
@@ -6508,16 +6508,16 @@
         <v>2</v>
       </c>
       <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.7565871912559727</v>
+      </c>
+      <c r="G9">
         <v>13</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0.7086330019615463</v>
-      </c>
-      <c r="G9">
-        <v>11</v>
       </c>
       <c r="H9">
         <v>10</v>
@@ -6555,7 +6555,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0.7561121106479907</v>
+        <v>0.7388936852715574</v>
       </c>
       <c r="G10">
         <v>10</v>
@@ -6590,16 +6590,16 @@
         <v>2</v>
       </c>
       <c r="D11">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0.7655374883431998</v>
+        <v>0.7422137537086848</v>
       </c>
       <c r="G11">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H11">
         <v>10</v>
@@ -6685,16 +6685,16 @@
         <v>41</v>
       </c>
       <c r="D2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.8024060459563362</v>
+        <v>0.8258279121365006</v>
       </c>
       <c r="G2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -6726,16 +6726,16 @@
         <v>41</v>
       </c>
       <c r="D3">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.8040076679140001</v>
+        <v>0.8019547939084266</v>
       </c>
       <c r="G3">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -6767,16 +6767,16 @@
         <v>41</v>
       </c>
       <c r="D4">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.8202418225548799</v>
+        <v>0.8038585972335438</v>
       </c>
       <c r="G4">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H4">
         <v>10</v>
@@ -6808,16 +6808,16 @@
         <v>41</v>
       </c>
       <c r="D5">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.8058925341342225</v>
+        <v>0.8096659244033756</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -6849,16 +6849,16 @@
         <v>41</v>
       </c>
       <c r="D6">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.8365332920813429</v>
+        <v>0.8022504593276011</v>
       </c>
       <c r="G6">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H6">
         <v>10</v>
@@ -6890,16 +6890,16 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.8021363251285796</v>
+        <v>0.8155868048226571</v>
       </c>
       <c r="G7">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7">
         <v>10</v>
@@ -6931,16 +6931,16 @@
         <v>2</v>
       </c>
       <c r="D8">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.8375216342451512</v>
+        <v>0.8053093810913493</v>
       </c>
       <c r="G8">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H8">
         <v>10</v>
@@ -6978,7 +6978,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.8127691948539225</v>
+        <v>0.8059327445559628</v>
       </c>
       <c r="G9">
         <v>18</v>
@@ -7019,7 +7019,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0.8321441117190954</v>
+        <v>0.8169413945696667</v>
       </c>
       <c r="G10">
         <v>13</v>
@@ -7054,16 +7054,16 @@
         <v>2</v>
       </c>
       <c r="D11">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0.8418152155039731</v>
+        <v>0.8111986099909742</v>
       </c>
       <c r="G11">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H11">
         <v>10</v>
@@ -7155,7 +7155,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.9512020154970848</v>
+        <v>0.9154578710470516</v>
       </c>
       <c r="G2">
         <v>21</v>
@@ -7190,16 +7190,16 @@
         <v>41</v>
       </c>
       <c r="D3">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.9006076888876728</v>
+        <v>0.9196757275380857</v>
       </c>
       <c r="G3">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -7237,7 +7237,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.9673247233641075</v>
+        <v>0.9173626100140798</v>
       </c>
       <c r="G4">
         <v>21</v>
@@ -7272,16 +7272,16 @@
         <v>41</v>
       </c>
       <c r="D5">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.9447972003991242</v>
+        <v>0.9130061602092915</v>
       </c>
       <c r="G5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -7319,7 +7319,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.9798226879535833</v>
+        <v>0.9407505842772275</v>
       </c>
       <c r="G6">
         <v>21</v>
@@ -7354,16 +7354,16 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.9039457816448612</v>
+        <v>0.9172913464676199</v>
       </c>
       <c r="G7">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H7">
         <v>10</v>
@@ -7401,7 +7401,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.9102205797229895</v>
+        <v>0.9006422998686134</v>
       </c>
       <c r="G8">
         <v>28</v>
@@ -7442,7 +7442,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.9302874451332112</v>
+        <v>0.9242432534333419</v>
       </c>
       <c r="G9">
         <v>22</v>
@@ -7477,16 +7477,16 @@
         <v>2</v>
       </c>
       <c r="D10">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0.9074864458438633</v>
+        <v>0.9266588642316403</v>
       </c>
       <c r="G10">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H10">
         <v>10</v>
@@ -7524,7 +7524,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0.9461142672866718</v>
+        <v>0.9627809043983722</v>
       </c>
       <c r="G11">
         <v>22</v>

</xml_diff>